<commit_message>
fixed requirements and mindmap
</commit_message>
<xml_diff>
--- a/Test stand test report May 2022 Andrey_Belyukin.xlsx
+++ b/Test stand test report May 2022 Andrey_Belyukin.xlsx
@@ -13,21 +13,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+  <si>
+    <t>№</t>
+  </si>
   <si>
     <t>Requirements</t>
   </si>
   <si>
+    <t xml:space="preserve">The start page should have input fields.
+1. Username
+2. Password
+Below should be a list - Accepted usernames are:
+    a) standard_user
+    b) locked_out_user
+    c) problem_user
+    d) performance_glitch_user
+And - Password for all users:
+    a) secret_sauce
+</t>
+  </si>
+  <si>
+    <t>Create sorting of goods according to the following criteria:
+1. A to Z
+2. Z to A
+3. Low to high
+4. High to low
+Sorting should be in the upper right corner</t>
+  </si>
+  <si>
+    <t>Create a shopping cart with this functionality:
+1. Add items to cart
+2. Remove items from the cart
+3. Collecting information about the client "CHECKOUT"
+      a) First Name
+      b)Last Name
+      c)Zip\Postal code
+4. After passing the "CHECKOUT" display a window with a confirmation of purchase</t>
+  </si>
+  <si>
+    <t>The site must be compatible with different operating systems and responsive design that adapts to different screen sizes and resolutions devices such as
+1. Windows 
+2. Android
+3. IOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Case Headers            </t>
   </si>
   <si>
-    <t xml:space="preserve">Functionality:
-1.User registration and login
-2.Product catalog with search and filtering capabilities
-3.Shopping cart for adding items and checking out
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that a sorting from "A to Z" working </t>
   </si>
   <si>
@@ -52,12 +85,6 @@
     <t xml:space="preserve">Verify that the products can be remove from the card </t>
   </si>
   <si>
-    <t>Design and usability:
-1.Clean and simple design that fits the store's theme
-2.Good navigation and user interface
-3.Fast page loading and minimal page transitions</t>
-  </si>
-  <si>
     <t>Verify that the price of the products is correct</t>
   </si>
   <si>
@@ -65,12 +92,6 @@
   </si>
   <si>
     <t>Verify that the description of the products is correct</t>
-  </si>
-  <si>
-    <t>Cross-platform:
-1.Compatibility with different operating systems and devices ( Windows, Android)
-2.Responsive design that adapts to different screen sizes and resolutions
-3.Consistent user experience across different platforms and devices</t>
   </si>
   <si>
     <t>Redmi note 5 UI test</t>
@@ -191,9 +212,6 @@
     <t>Price is the same "29.99"</t>
   </si>
   <si>
-    <t>№</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -291,10 +309,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -311,6 +335,11 @@
     </font>
     <font/>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -324,11 +353,6 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -472,92 +496,111 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -588,7 +631,7 @@
     <xdr:ext cx="2762250" cy="5495925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -644,7 +687,7 @@
     <xdr:ext cx="2752725" cy="5495925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Изображение"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Изображение"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -871,354 +914,412 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="7.63"/>
     <col customWidth="1" min="2" max="2" width="47.13"/>
-    <col customWidth="1" min="3" max="3" width="54.5"/>
-    <col customWidth="1" min="4" max="4" width="7.63"/>
-    <col customWidth="1" min="5" max="5" width="11.75"/>
-    <col customWidth="1" min="6" max="25" width="7.63"/>
+    <col customWidth="1" min="3" max="3" width="16.0"/>
+    <col customWidth="1" min="4" max="4" width="8.5"/>
+    <col customWidth="1" min="5" max="5" width="7.63"/>
+    <col customWidth="1" min="6" max="6" width="11.75"/>
+    <col customWidth="1" min="7" max="26" width="7.63"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" customHeight="1">
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="16.5" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" ht="18.0" customHeight="1">
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" ht="23.25" customHeight="1">
+      <c r="A2" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" ht="21.0" customHeight="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" ht="22.5" customHeight="1">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" ht="25.5" customHeight="1">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" ht="15.0" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="14">
+        <v>3.0</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" ht="21.75" customHeight="1">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" ht="52.5" customHeight="1">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" ht="87.75" customHeight="1">
+      <c r="A16" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="4"/>
-      <c r="C6" s="6" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="4"/>
-      <c r="C7" s="6" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="4"/>
-      <c r="C8" s="6" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="7"/>
-      <c r="C9" s="6" t="s">
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="8" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" ht="21.75" customHeight="1">
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" ht="20.25" customHeight="1">
-      <c r="B12" s="7"/>
-      <c r="C12" s="3" t="s">
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" ht="24.75" customHeight="1">
-      <c r="B13" s="8" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" ht="23.25" customHeight="1">
-      <c r="B14" s="4"/>
-      <c r="C14" s="3" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" ht="21.75" customHeight="1">
-      <c r="B15" s="7"/>
-      <c r="C15" s="3" t="s">
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31">
+      <c r="B31" s="17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27">
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28">
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32">
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
     </row>
     <row r="33">
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
     </row>
     <row r="34">
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
     </row>
     <row r="35">
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
     </row>
     <row r="36">
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
     </row>
     <row r="37">
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
     </row>
     <row r="38">
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
     </row>
     <row r="39">
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
     </row>
     <row r="40">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
     </row>
     <row r="41">
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
     </row>
     <row r="42">
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43">
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
     </row>
     <row r="44">
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
     </row>
     <row r="45">
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
     </row>
     <row r="46">
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
     </row>
     <row r="47">
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
     </row>
     <row r="48">
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
     </row>
     <row r="49">
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
     </row>
     <row r="50">
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
     </row>
     <row r="51">
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
     </row>
     <row r="52">
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
     </row>
     <row r="53">
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
     </row>
     <row r="54">
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
     </row>
     <row r="55">
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
     </row>
     <row r="56">
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
     </row>
     <row r="57">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
     </row>
     <row r="58">
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
     </row>
     <row r="59">
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
     </row>
     <row r="60">
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
     </row>
     <row r="61">
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
     </row>
     <row r="62">
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
     </row>
     <row r="63">
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
     </row>
     <row r="64">
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-    </row>
-    <row r="65">
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-    </row>
-    <row r="66">
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-    </row>
-    <row r="67">
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-    </row>
-    <row r="68">
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-    </row>
-    <row r="69">
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-    </row>
-    <row r="70">
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
-    </row>
-    <row r="71">
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-    </row>
-    <row r="72">
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
-    </row>
-    <row r="73">
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-    </row>
-    <row r="74">
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-    </row>
-    <row r="75">
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-    </row>
-    <row r="76">
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-    </row>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+    </row>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
     <row r="77"/>
     <row r="78"/>
     <row r="79"/>
@@ -2123,23 +2224,12 @@
     <row r="978"/>
     <row r="979"/>
     <row r="980"/>
-    <row r="981"/>
-    <row r="982"/>
-    <row r="983"/>
-    <row r="984"/>
-    <row r="985"/>
-    <row r="986"/>
-    <row r="987"/>
-    <row r="988"/>
-    <row r="989"/>
-    <row r="990"/>
-    <row r="991"/>
-    <row r="992"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+  <mergeCells count="4">
     <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A11:A15"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2165,244 +2255,244 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12"/>
+      <c r="A1" s="19"/>
     </row>
     <row r="2">
-      <c r="A2" s="12"/>
+      <c r="A2" s="19"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="20"/>
+      <c r="B6" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="20"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="20"/>
+      <c r="B8" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="20"/>
+      <c r="B9" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="20"/>
+      <c r="B10" s="33">
+        <v>2.0</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="20"/>
+      <c r="B11" s="30">
+        <v>3.0</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="20"/>
+      <c r="B12" s="33">
+        <v>4.0</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
+      <c r="C14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="K14" s="37"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="13"/>
-      <c r="B6" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="13"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="13"/>
-      <c r="B8" s="22" t="s">
+      <c r="C15" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="C19" s="29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="13"/>
-      <c r="B9" s="23">
+      <c r="D19" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="30">
         <v>1.0</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="25" t="s">
+      <c r="C20" s="32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="13"/>
-      <c r="B10" s="26">
+      <c r="D20" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="33">
         <v>2.0</v>
       </c>
-      <c r="C10" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="28" t="s">
+      <c r="C21" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="13"/>
-      <c r="B11" s="23">
+    </row>
+    <row r="22">
+      <c r="B22" s="30">
         <v>3.0</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="13"/>
-      <c r="B12" s="26">
+      <c r="C22" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="33">
         <v>4.0</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
-      <c r="K14" s="30"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="23">
-        <v>1.0</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="23">
-        <v>3.0</v>
-      </c>
-      <c r="C22" s="29" t="s">
+      <c r="C23" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" s="26">
-        <v>4.0</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>31</v>
+      <c r="D23" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2444,97 +2534,97 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="31" t="s">
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="C1" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="D1" s="38" t="s">
         <v>50</v>
       </c>
+      <c r="E1" s="38" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="32">
+      <c r="A2" s="39">
         <v>1.0</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="C2" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="D2" s="39" t="s">
         <v>54</v>
       </c>
+      <c r="E2" s="39" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="32">
+      <c r="A3" s="39">
         <v>2.0</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="C3" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="D3" s="39" t="s">
         <v>58</v>
       </c>
+      <c r="E3" s="39" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="32">
+      <c r="A4" s="39">
         <v>3.0</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="32" t="s">
+      <c r="B4" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="D4" s="39" t="s">
         <v>62</v>
       </c>
+      <c r="E4" s="39" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="32">
+      <c r="A5" s="39">
         <v>4.0</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="39" t="s">
         <v>66</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6"/>
     <row r="7"/>
     <row r="8"/>
     <row r="9">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34" t="s">
-        <v>67</v>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10"/>

</xml_diff>